<commit_message>
input bug fixed, lesson 3 exercises completed
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_fillitin_exercise.xlsx
+++ b/public/docs/Grammar_fillitin_exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DDB24F-3F5A-4735-8867-662A9523BAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD15242-D3B1-4495-B8D8-6A56C85A980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2550" windowWidth="29040" windowHeight="15720" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView xWindow="792" yWindow="576" windowWidth="13896" windowHeight="11556" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="64">
   <si>
     <t>beginning text</t>
   </si>
@@ -168,6 +168,66 @@
   </si>
   <si>
     <t>{sentence: "</t>
+  </si>
+  <si>
+    <t>Він завжди миє свої руки перед обідом</t>
+  </si>
+  <si>
+    <t>Вони допомагають своїм друзям</t>
+  </si>
+  <si>
+    <t>He always washes his hands before dinner</t>
+  </si>
+  <si>
+    <t>They help their friends</t>
+  </si>
+  <si>
+    <t>Я ходжу в зал по понеділкам</t>
+  </si>
+  <si>
+    <t>I go to the gym on Mondays</t>
+  </si>
+  <si>
+    <t>Вона працює в магазині</t>
+  </si>
+  <si>
+    <t>Мій батько бігає вранці</t>
+  </si>
+  <si>
+    <t>Її син любить гратися</t>
+  </si>
+  <si>
+    <t>У йьому місці подають гарну каву</t>
+  </si>
+  <si>
+    <t>Мені потрібна інша ручка</t>
+  </si>
+  <si>
+    <t>Ми їздимо на тому ж автобусі кожного ранку</t>
+  </si>
+  <si>
+    <t>We take the same bus every morning</t>
+  </si>
+  <si>
+    <t>You must think about your health</t>
+  </si>
+  <si>
+    <t>Ви мусите подумати про здоров'я</t>
+  </si>
+  <si>
+    <t>I need another pen</t>
+  </si>
+  <si>
+    <t>She works in the store</t>
+  </si>
+  <si>
+    <t>Her son loves to play</t>
+  </si>
+  <si>
+    <t>My father runs in the mornings</t>
+  </si>
+  <si>
+    <t>This place serves good coffee</t>
   </si>
 </sst>
 </file>
@@ -577,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
   <dimension ref="A2:F360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1045,18 +1105,21 @@
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Він завжди миє свої руки перед обідом", translat: "He always washes his hands before dinner"},</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1064,20 +1127,20 @@
         <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Вони допомагають своїм друзям", translat: "They help their friends"},</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1085,20 +1148,20 @@
         <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Я ходжу в зал по понеділкам", translat: "I go to the gym on Mondays"},</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1106,20 +1169,20 @@
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Вона працює в магазині", translat: "She works in the store"},</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1127,20 +1190,20 @@
         <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Її син любить гратися", translat: "Her son loves to play"},</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1148,20 +1211,20 @@
         <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Мій батько бігає вранці", translat: "My father runs in the mornings"},</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1169,20 +1232,20 @@
         <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "У йьому місці подають гарну каву", translat: "This place serves good coffee"},</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1190,20 +1253,20 @@
         <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Мені потрібна інша ручка", translat: "I need another pen"},</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1211,20 +1274,20 @@
         <v>43</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Ви мусите подумати про здоров'я", translat: "You must think about your health"},</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1232,20 +1295,20 @@
         <v>43</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Ми їздимо на тому ж автобусі кожного ранку", translat: "We take the same bus every morning"},</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
lesson 4 exercises completed
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_fillitin_exercise.xlsx
+++ b/public/docs/Grammar_fillitin_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD15242-D3B1-4495-B8D8-6A56C85A980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E11824D-7445-42D0-884B-54CA67FA234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="576" windowWidth="13896" windowHeight="11556" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView xWindow="-396" yWindow="1140" windowWidth="15372" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="84">
   <si>
     <t>beginning text</t>
   </si>
@@ -228,6 +228,66 @@
   </si>
   <si>
     <t>This place serves good coffee</t>
+  </si>
+  <si>
+    <t>Ми зараз почнемо збори</t>
+  </si>
+  <si>
+    <t>Вона подвонить тобі на перерві</t>
+  </si>
+  <si>
+    <t>Ти багато вивчиш у цьому курсі</t>
+  </si>
+  <si>
+    <t>Вони прибудуть біля 6 вечора</t>
+  </si>
+  <si>
+    <t>Джон залишиться на роботі допізна</t>
+  </si>
+  <si>
+    <t>Він сформує нову команду</t>
+  </si>
+  <si>
+    <t>Я приготую м'со на вечерю</t>
+  </si>
+  <si>
+    <t>Повітря буде відчуватися холоднішим</t>
+  </si>
+  <si>
+    <t>Wt will spend the day together</t>
+  </si>
+  <si>
+    <t>Ми проведемо день разом</t>
+  </si>
+  <si>
+    <t>The air will feel cooler</t>
+  </si>
+  <si>
+    <t>We will start the meeting now</t>
+  </si>
+  <si>
+    <t>She will call you during the break</t>
+  </si>
+  <si>
+    <t>You will learn a lot in this course</t>
+  </si>
+  <si>
+    <t>They will arrive around 6p.m.</t>
+  </si>
+  <si>
+    <t>John will stay late at work</t>
+  </si>
+  <si>
+    <t>He will form a new team</t>
+  </si>
+  <si>
+    <t>I will cook meat for dinner</t>
+  </si>
+  <si>
+    <t>She will visit this place again</t>
+  </si>
+  <si>
+    <t>Вона відвідає це місце знову</t>
   </si>
 </sst>
 </file>
@@ -637,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
   <dimension ref="A2:F360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1330,18 +1390,21 @@
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B39" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Ми зараз почнемо збори", translat: "We will start the meeting now"},</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1349,20 +1412,20 @@
         <v>43</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Вона подвонить тобі на перерві", translat: "She will call you during the break"},</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1370,20 +1433,20 @@
         <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Ти багато вивчиш у цьому курсі", translat: "You will learn a lot in this course"},</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1391,20 +1454,20 @@
         <v>43</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Вони прибудуть біля 6 вечора", translat: "They will arrive around 6p.m."},</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1412,20 +1475,20 @@
         <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Джон залишиться на роботі допізна", translat: "John will stay late at work"},</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1433,20 +1496,20 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Він сформує нову команду", translat: "He will form a new team"},</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1454,20 +1517,20 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Я приготую м'со на вечерю", translat: "I will cook meat for dinner"},</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1475,20 +1538,20 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Вона відвідає це місце знову", translat: "She will visit this place again"},</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,20 +1559,20 @@
         <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Повітря буде відчуватися холоднішим", translat: "The air will feel cooler"},</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,20 +1580,20 @@
         <v>43</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F48" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Ми проведемо день разом", translat: "Wt will spend the day together"},</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fillitin exercises finished for 9 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_fillitin_exercise.xlsx
+++ b/public/docs/Grammar_fillitin_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E11824D-7445-42D0-884B-54CA67FA234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B331B639-72B5-4241-9B8B-180ACADBC213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-396" yWindow="1140" windowWidth="15372" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView xWindow="48" yWindow="1068" windowWidth="14292" windowHeight="10008" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="184">
   <si>
     <t>beginning text</t>
   </si>
@@ -288,6 +288,306 @@
   </si>
   <si>
     <t>Вона відвідає це місце знову</t>
+  </si>
+  <si>
+    <t>He finished the project on time</t>
+  </si>
+  <si>
+    <t>They played soccer in the park</t>
+  </si>
+  <si>
+    <t>We collected the information last week</t>
+  </si>
+  <si>
+    <t>She talked less during the meeting</t>
+  </si>
+  <si>
+    <t>I typed the letter</t>
+  </si>
+  <si>
+    <t>She turned off the lights</t>
+  </si>
+  <si>
+    <t>He missed her wife very much</t>
+  </si>
+  <si>
+    <t>I watched him going away</t>
+  </si>
+  <si>
+    <t>They prepared the report before the deadline</t>
+  </si>
+  <si>
+    <t>Вона говорила меньше перед зустріччю</t>
+  </si>
+  <si>
+    <t>Вони грали у футбол в дворі</t>
+  </si>
+  <si>
+    <t>Він закінчив проект вчасно</t>
+  </si>
+  <si>
+    <t>Ми зібрали інформацію минулого тижня</t>
+  </si>
+  <si>
+    <t>Я надрукував листа</t>
+  </si>
+  <si>
+    <t>Вона вимкнула світло</t>
+  </si>
+  <si>
+    <t>Він скучив за дружиною дуже сильно</t>
+  </si>
+  <si>
+    <t>Вони підготували звіт перед дедлайном</t>
+  </si>
+  <si>
+    <t>Я дивився, як він йде геть</t>
+  </si>
+  <si>
+    <t>Ми приготували їжу для всієї сім'ї</t>
+  </si>
+  <si>
+    <t>We cooked food for the whole family</t>
+  </si>
+  <si>
+    <t>I met my friend at the café</t>
+  </si>
+  <si>
+    <t>He put his keys on the table</t>
+  </si>
+  <si>
+    <t>She sold her old bicycle</t>
+  </si>
+  <si>
+    <t>I sent the email last night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The children sang a song at the school </t>
+  </si>
+  <si>
+    <t>He took a photo of the sunset</t>
+  </si>
+  <si>
+    <t>I woke up early today</t>
+  </si>
+  <si>
+    <t>She wrote a letter to her grandmother</t>
+  </si>
+  <si>
+    <t>Я зустрів свого друга в кафе</t>
+  </si>
+  <si>
+    <t>Він поклав ключі на стіл</t>
+  </si>
+  <si>
+    <t>Вони пробігли 5 миль вранці</t>
+  </si>
+  <si>
+    <t>They ran 5 miles in the morning</t>
+  </si>
+  <si>
+    <t>Вона прочитала 3 книги</t>
+  </si>
+  <si>
+    <t>She read 3 books</t>
+  </si>
+  <si>
+    <t>Вона продала свій старий велосипед</t>
+  </si>
+  <si>
+    <t>Я відправив емейл вчора ввечері</t>
+  </si>
+  <si>
+    <t>Діти співали пісню в школі</t>
+  </si>
+  <si>
+    <t>Він зняв фото заходу сонця</t>
+  </si>
+  <si>
+    <t>Я прокинувся рано сьогодні</t>
+  </si>
+  <si>
+    <t>Вона написала листа бабусі</t>
+  </si>
+  <si>
+    <t>Will you set the alarm?</t>
+  </si>
+  <si>
+    <t>Did the birds sing in the morning?</t>
+  </si>
+  <si>
+    <t>Does she work as a guide?</t>
+  </si>
+  <si>
+    <t>Will the teacher help the students?</t>
+  </si>
+  <si>
+    <t>Do seasons change every 4 months?</t>
+  </si>
+  <si>
+    <t>Does music interest many people?</t>
+  </si>
+  <si>
+    <t>Did he study literature at university?</t>
+  </si>
+  <si>
+    <t>Do you walk to work?</t>
+  </si>
+  <si>
+    <t>Will we solve the problem together?</t>
+  </si>
+  <si>
+    <t>Do they say hello every day?</t>
+  </si>
+  <si>
+    <t>Ти поставиш будильник?</t>
+  </si>
+  <si>
+    <t>Чи співали пташки вранці?</t>
+  </si>
+  <si>
+    <t>Вона працює гідом?</t>
+  </si>
+  <si>
+    <t>Чи допоможе вчитель студентам?</t>
+  </si>
+  <si>
+    <t>Чи змініються сезони кожні 4 місяці?</t>
+  </si>
+  <si>
+    <t>Чи цікавить музика багатьох людей?</t>
+  </si>
+  <si>
+    <t>Чи вивчав він літературу в університеті?</t>
+  </si>
+  <si>
+    <t>Ви ходите пішки на роботу?</t>
+  </si>
+  <si>
+    <t>Ми вирішимо проблему разом?</t>
+  </si>
+  <si>
+    <t>Чи вітаються вони кожного дня?</t>
+  </si>
+  <si>
+    <t>She will be listening to the concert</t>
+  </si>
+  <si>
+    <t>We will be talking about it tomorrow</t>
+  </si>
+  <si>
+    <t>They will be checking the size</t>
+  </si>
+  <si>
+    <t>I will be moving next month</t>
+  </si>
+  <si>
+    <t>He will be building a big house</t>
+  </si>
+  <si>
+    <t>We will be doing everything possible</t>
+  </si>
+  <si>
+    <t>They will be watching TV</t>
+  </si>
+  <si>
+    <t>You will be learning it next week</t>
+  </si>
+  <si>
+    <t>The teacher will be explaining the new topic</t>
+  </si>
+  <si>
+    <t>The ladies will be drinking wine</t>
+  </si>
+  <si>
+    <t>Пані будуть пити вино</t>
+  </si>
+  <si>
+    <t>Вона слухатиме концерт</t>
+  </si>
+  <si>
+    <t>Ми будемо говорити про це завтра</t>
+  </si>
+  <si>
+    <t>Вони перевірятимуть розмір</t>
+  </si>
+  <si>
+    <t>Я переїжджатиму наступного місяця</t>
+  </si>
+  <si>
+    <t>Він будуватиме великий будинок</t>
+  </si>
+  <si>
+    <t>Ми робитимемо все можливе</t>
+  </si>
+  <si>
+    <t>Вони дивитимуться телевізор</t>
+  </si>
+  <si>
+    <t>Ви вивчатимете це наступного тижня</t>
+  </si>
+  <si>
+    <t>Вчитель пояснюватиме нову тему</t>
+  </si>
+  <si>
+    <t>Is she working late these days?</t>
+  </si>
+  <si>
+    <t>Were they celebrating a holday today?</t>
+  </si>
+  <si>
+    <t>Is he improving his level of English?</t>
+  </si>
+  <si>
+    <t>Were you placing the order?</t>
+  </si>
+  <si>
+    <t>Will the students be practicing?</t>
+  </si>
+  <si>
+    <t>Are the scientists conducting research?</t>
+  </si>
+  <si>
+    <t>Were people feeling hot yesterday?</t>
+  </si>
+  <si>
+    <t>Is she using text messages?</t>
+  </si>
+  <si>
+    <t>Чи працює вона допізна цими днями?</t>
+  </si>
+  <si>
+    <t>Вони відмічали свято сьогодні?</t>
+  </si>
+  <si>
+    <t>Чи зменьшуватиме компанія відходи?</t>
+  </si>
+  <si>
+    <t>Will company be reducing the waste?</t>
+  </si>
+  <si>
+    <t>Він покращує рівень англійської?</t>
+  </si>
+  <si>
+    <t>Ви розміщували замовлення?</t>
+  </si>
+  <si>
+    <t>Чи практикуватимуться студенти?</t>
+  </si>
+  <si>
+    <t>Чи проводять вчені дослідження?</t>
+  </si>
+  <si>
+    <t>Чи було спекотно людям вчора?</t>
+  </si>
+  <si>
+    <t>Вона користується смсками?</t>
+  </si>
+  <si>
+    <t>Чи робитимуть вони 3 проекти?</t>
+  </si>
+  <si>
+    <t>Will they be doing 3 projects?</t>
   </si>
 </sst>
 </file>
@@ -697,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
   <dimension ref="A2:F360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="E96" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99:F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1615,18 +1915,21 @@
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B51" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="C51" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Вона говорила меньше перед зустріччю", translat: "She talked less during the meeting"},</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1634,20 +1937,20 @@
         <v>43</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F52" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Вони грали у футбол в дворі", translat: "They played soccer in the park"},</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1655,20 +1958,20 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F53" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Він закінчив проект вчасно", translat: "He finished the project on time"},</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,20 +1979,20 @@
         <v>43</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F54" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Ми зібрали інформацію минулого тижня", translat: "We collected the information last week"},</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1697,20 +2000,20 @@
         <v>43</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F55" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Я надрукував листа", translat: "I typed the letter"},</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1718,20 +2021,20 @@
         <v>43</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F56" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Вона вимкнула світло", translat: "She turned off the lights"},</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1739,20 +2042,20 @@
         <v>43</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F57" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Він скучив за дружиною дуже сильно", translat: "He missed her wife very much"},</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1760,20 +2063,20 @@
         <v>43</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F58" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Вони підготували звіт перед дедлайном", translat: "They prepared the report before the deadline"},</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1781,20 +2084,20 @@
         <v>43</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F59" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Я дивився, як він йде геть", translat: "I watched him going away"},</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,20 +2105,20 @@
         <v>43</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F60" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Ми приготували їжу для всієї сім'ї", translat: "We cooked food for the whole family"},</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1837,18 +2140,21 @@
       <c r="A63" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B63" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="C63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F63" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Я зустрів свого друга в кафе", translat: "I met my friend at the café"},</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,20 +2162,20 @@
         <v>43</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F64" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Вона прочитала 3 книги", translat: "She read 3 books"},</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,20 +2183,20 @@
         <v>43</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F65" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Він поклав ключі на стіл", translat: "He put his keys on the table"},</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1898,20 +2204,20 @@
         <v>43</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F66" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Вони пробігли 5 миль вранці", translat: "They ran 5 miles in the morning"},</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1919,20 +2225,20 @@
         <v>43</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F67" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Вона продала свій старий велосипед", translat: "She sold her old bicycle"},</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1940,20 +2246,20 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F68" s="2" t="str">
         <f t="shared" ref="F68:F131" si="1">A68&amp;B68&amp;C68&amp;D68&amp;E68</f>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Я відправив емейл вчора ввечері", translat: "I sent the email last night"},</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1961,20 +2267,20 @@
         <v>43</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F69" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Діти співали пісню в школі", translat: "The children sang a song at the school "},</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,20 +2288,20 @@
         <v>43</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F70" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Він зняв фото заходу сонця", translat: "He took a photo of the sunset"},</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2003,20 +2309,20 @@
         <v>43</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F71" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Я прокинувся рано сьогодні", translat: "I woke up early today"},</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2024,20 +2330,20 @@
         <v>43</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F72" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Вона написала листа бабусі", translat: "She wrote a letter to her grandmother"},</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2059,18 +2365,21 @@
       <c r="A75" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B75" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="C75" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F75" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Ти поставиш будильник?", translat: "Will you set the alarm?"},</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2078,20 +2387,20 @@
         <v>43</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F76" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Чи співали пташки вранці?", translat: "Did the birds sing in the morning?"},</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2099,20 +2408,20 @@
         <v>43</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F77" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Вона працює гідом?", translat: "Does she work as a guide?"},</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2120,20 +2429,20 @@
         <v>43</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F78" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Чи допоможе вчитель студентам?", translat: "Will the teacher help the students?"},</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2141,20 +2450,20 @@
         <v>43</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F79" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Чи змініються сезони кожні 4 місяці?", translat: "Do seasons change every 4 months?"},</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2162,20 +2471,20 @@
         <v>43</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F80" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Чи цікавить музика багатьох людей?", translat: "Does music interest many people?"},</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2183,20 +2492,20 @@
         <v>43</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F81" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Чи вивчав він літературу в університеті?", translat: "Did he study literature at university?"},</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,20 +2513,20 @@
         <v>43</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F82" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Ви ходите пішки на роботу?", translat: "Do you walk to work?"},</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,20 +2534,20 @@
         <v>43</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F83" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Ми вирішимо проблему разом?", translat: "Will we solve the problem together?"},</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2246,20 +2555,20 @@
         <v>43</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F84" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Чи вітаються вони кожного дня?", translat: "Do they say hello every day?"},</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2281,18 +2590,21 @@
       <c r="A87" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B87" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="C87" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F87" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Вона слухатиме концерт", translat: "She will be listening to the concert"},</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2300,20 +2612,20 @@
         <v>43</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F88" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Ми будемо говорити про це завтра", translat: "We will be talking about it tomorrow"},</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2321,20 +2633,20 @@
         <v>43</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F89" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Вони перевірятимуть розмір", translat: "They will be checking the size"},</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2342,20 +2654,20 @@
         <v>43</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F90" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Я переїжджатиму наступного місяця", translat: "I will be moving next month"},</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,20 +2675,20 @@
         <v>43</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F91" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Він будуватиме великий будинок", translat: "He will be building a big house"},</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2384,20 +2696,20 @@
         <v>43</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>9</v>
+        <v>149</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F92" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Ми робитимемо все можливе", translat: "We will be doing everything possible"},</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2405,20 +2717,20 @@
         <v>43</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F93" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Вони дивитимуться телевізор", translat: "They will be watching TV"},</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2426,20 +2738,20 @@
         <v>43</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>11</v>
+        <v>151</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F94" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Ви вивчатимете це наступного тижня", translat: "You will be learning it next week"},</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2447,20 +2759,20 @@
         <v>43</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F95" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Вчитель пояснюватиме нову тему", translat: "The teacher will be explaining the new topic"},</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2468,20 +2780,20 @@
         <v>43</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F96" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Пані будуть пити вино", translat: "The ladies will be drinking wine"},</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2503,18 +2815,21 @@
       <c r="A99" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B99" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="C99" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F99" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "", translat: "Я"},</v>
+        <v>{sentence: "Чи працює вона допізна цими днями?", translat: "Is she working late these days?"},</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,20 +2837,20 @@
         <v>43</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>3</v>
+        <v>165</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F100" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text2"},</v>
+        <v>{sentence: "Вони відмічали свято сьогодні?", translat: "Were they celebrating a holday today?"},</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2543,20 +2858,20 @@
         <v>43</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F101" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text3"},</v>
+        <v>{sentence: "Чи зменьшуватиме компанія відходи?", translat: "Will company be reducing the waste?"},</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2564,20 +2879,20 @@
         <v>43</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F102" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text4"},</v>
+        <v>{sentence: "Він покращує рівень англійської?", translat: "Is he improving his level of English?"},</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2585,20 +2900,20 @@
         <v>43</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F103" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text5"},</v>
+        <v>{sentence: "Ви розміщували замовлення?", translat: "Were you placing the order?"},</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,20 +2921,20 @@
         <v>43</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F104" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text6"},</v>
+        <v>{sentence: "Чи практикуватимуться студенти?", translat: "Will the students be practicing?"},</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2627,20 +2942,20 @@
         <v>43</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F105" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text7"},</v>
+        <v>{sentence: "Чи проводять вчені дослідження?", translat: "Are the scientists conducting research?"},</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,20 +2963,20 @@
         <v>43</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F106" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text8"},</v>
+        <v>{sentence: "Чи було спекотно людям вчора?", translat: "Were people feeling hot yesterday?"},</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2669,20 +2984,20 @@
         <v>43</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F107" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text9"},</v>
+        <v>{sentence: "Вона користується смсками?", translat: "Is she using text messages?"},</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2690,20 +3005,20 @@
         <v>43</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>13</v>
+        <v>183</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F108" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{sentence: "beginning text", translat: "word text10"},</v>
+        <v>{sentence: "Чи робитимуть вони 3 проекти?", translat: "Will they be doing 3 projects?"},</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>